<commit_message>
null/del filter works, but json wont be created
</commit_message>
<xml_diff>
--- a/src/main/resources/importfiles/company/temp_masterinput/RND_Std_032023_sample_problems.xlsx
+++ b/src/main/resources/importfiles/company/temp_masterinput/RND_Std_032023_sample_problems.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26501"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\otter\Documents\CoderBay\baetter\baetter-identifier\src\main\resources\importfiles\testfiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Eigene Dateien\Dokumente\GitHub\Baetter-Solutions\baetter-identifier\src\main\resources\importfiles\company\temp_masterinput\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{920C6FB2-92FA-4C58-8136-DD3EC8EEF0CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{578AF9E1-91AE-42E5-9455-F76C2E63E3DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{23498E98-C16E-46DF-AD53-14088726713D}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{23498E98-C16E-46DF-AD53-14088726713D}"/>
   </bookViews>
   <sheets>
     <sheet name="full" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="97">
   <si>
     <t>ARTIKELNUMMER</t>
   </si>
@@ -86,27 +86,12 @@
     <t>400194</t>
   </si>
   <si>
-    <t>ABB</t>
-  </si>
-  <si>
     <t>AB.A1</t>
   </si>
   <si>
-    <t>ZLS840 K.mod. 1f DIN Schiene</t>
-  </si>
-  <si>
-    <t>K.mod. 1f DIN Schiene ZLS840</t>
-  </si>
-  <si>
     <t>2CCA180450R0001</t>
   </si>
   <si>
-    <t>ZLS8403LABWT-S</t>
-  </si>
-  <si>
-    <t>K.mod. ZLS8403LABWT-S 1f</t>
-  </si>
-  <si>
     <t>2CCA180453R0001</t>
   </si>
   <si>
@@ -275,24 +260,12 @@
     <t>7612270109074</t>
   </si>
   <si>
-    <t>K.mod. ZLS840LAB-X3 La/Lb</t>
-  </si>
-  <si>
-    <t>ZLS840LAB-X3</t>
-  </si>
-  <si>
     <t>120753970</t>
   </si>
   <si>
     <t>120753968</t>
   </si>
   <si>
-    <t>ZLS8403LWT-S</t>
-  </si>
-  <si>
-    <t>Kombimodul ZLS8403LWT-S 1f</t>
-  </si>
-  <si>
     <t>7612270054053</t>
   </si>
   <si>
@@ -341,7 +314,19 @@
     <t>0</t>
   </si>
   <si>
-    <t>TESTARTIKEL</t>
+    <t>Artikel entfernt</t>
+  </si>
+  <si>
+    <t>AX Nummer fehlt</t>
+  </si>
+  <si>
+    <t>PE fehlt</t>
+  </si>
+  <si>
+    <t>Preis ist leer</t>
+  </si>
+  <si>
+    <t>ALLES PASST</t>
   </si>
 </sst>
 </file>
@@ -694,7 +679,7 @@
   <dimension ref="A1:AP6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P7" sqref="P7"/>
+      <selection activeCell="P5" sqref="P5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -713,7 +698,7 @@
         <v>2</v>
       </c>
       <c r="E1" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>3</v>
@@ -722,177 +707,177 @@
         <v>4</v>
       </c>
       <c r="H1" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="I1" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="J1" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="K1" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="L1" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="M1" s="2" t="s">
         <v>5</v>
       </c>
       <c r="N1" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="O1" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="P1" s="2" t="s">
         <v>6</v>
       </c>
       <c r="Q1" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="R1" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="S1" s="3" t="s">
         <v>7</v>
       </c>
       <c r="T1" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="U1" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="V1" s="3" t="s">
         <v>8</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="X1" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="Y1" s="2" t="s">
         <v>9</v>
       </c>
       <c r="Z1" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="AA1" s="2" t="s">
         <v>10</v>
       </c>
       <c r="AB1" t="s">
+        <v>53</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>57</v>
+      </c>
+      <c r="AG1" t="s">
         <v>58</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AH1" t="s">
         <v>59</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AI1" t="s">
         <v>60</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AJ1" t="s">
         <v>61</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AK1" t="s">
         <v>62</v>
-      </c>
-      <c r="AG1" t="s">
-        <v>63</v>
-      </c>
-      <c r="AH1" t="s">
-        <v>64</v>
-      </c>
-      <c r="AI1" t="s">
-        <v>65</v>
-      </c>
-      <c r="AJ1" t="s">
-        <v>66</v>
-      </c>
-      <c r="AK1" t="s">
-        <v>67</v>
       </c>
       <c r="AL1" s="2" t="s">
         <v>11</v>
       </c>
       <c r="AM1" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="AN1" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="AO1" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="AP1" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
     </row>
     <row r="2" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="B2">
         <v>120753970</v>
       </c>
       <c r="C2" t="s">
-        <v>80</v>
+        <v>92</v>
       </c>
       <c r="D2" t="s">
-        <v>79</v>
+        <v>92</v>
       </c>
       <c r="E2" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="F2" t="s">
         <v>15</v>
       </c>
       <c r="G2" t="s">
+        <v>92</v>
+      </c>
+      <c r="H2" t="s">
+        <v>70</v>
+      </c>
+      <c r="I2" t="s">
+        <v>72</v>
+      </c>
+      <c r="J2" t="s">
+        <v>71</v>
+      </c>
+      <c r="M2" t="s">
         <v>16</v>
       </c>
-      <c r="H2" t="s">
-        <v>75</v>
-      </c>
-      <c r="I2" t="s">
-        <v>77</v>
-      </c>
-      <c r="J2" t="s">
-        <v>76</v>
-      </c>
-      <c r="M2" t="s">
-        <v>17</v>
-      </c>
       <c r="N2" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="O2" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="P2" t="s">
-        <v>75</v>
+        <v>92</v>
       </c>
       <c r="Q2" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="R2" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="S2" s="1">
-        <v>84.4</v>
+        <v>100</v>
       </c>
       <c r="T2" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="U2" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="V2" s="4" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="W2" s="1" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="X2" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="Y2" t="s">
         <v>13</v>
@@ -907,94 +892,94 @@
         <v>12</v>
       </c>
       <c r="AD2" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="AE2" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="AG2" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="AH2" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="AI2" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="AL2" t="s">
         <v>12</v>
       </c>
       <c r="AN2" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="AP2" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
     </row>
     <row r="3" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B3" s="6"/>
       <c r="C3" t="s">
-        <v>18</v>
+        <v>93</v>
       </c>
       <c r="D3" t="s">
-        <v>19</v>
+        <v>93</v>
       </c>
       <c r="E3" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="F3" t="s">
         <v>15</v>
       </c>
       <c r="G3" t="s">
+        <v>93</v>
+      </c>
+      <c r="H3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I3" t="s">
+        <v>30</v>
+      </c>
+      <c r="J3" t="s">
+        <v>23</v>
+      </c>
+      <c r="M3" t="s">
         <v>16</v>
       </c>
-      <c r="H3" t="s">
-        <v>20</v>
-      </c>
-      <c r="I3" t="s">
-        <v>35</v>
-      </c>
-      <c r="J3" t="s">
+      <c r="N3" t="s">
+        <v>24</v>
+      </c>
+      <c r="O3" t="s">
+        <v>25</v>
+      </c>
+      <c r="P3" t="s">
+        <v>93</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>26</v>
+      </c>
+      <c r="R3" t="s">
+        <v>27</v>
+      </c>
+      <c r="S3" s="1">
+        <v>200</v>
+      </c>
+      <c r="T3" t="s">
         <v>28</v>
       </c>
-      <c r="M3" t="s">
-        <v>17</v>
-      </c>
-      <c r="N3" t="s">
-        <v>29</v>
-      </c>
-      <c r="O3" t="s">
-        <v>30</v>
-      </c>
-      <c r="P3" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>31</v>
-      </c>
-      <c r="R3" t="s">
-        <v>32</v>
-      </c>
-      <c r="S3" s="1">
-        <v>44.7</v>
-      </c>
-      <c r="T3" t="s">
-        <v>33</v>
-      </c>
       <c r="U3" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="V3" s="1">
         <v>30.549999999999997</v>
       </c>
       <c r="W3" s="1" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="X3" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="Y3" t="s">
         <v>13</v>
@@ -1009,102 +994,102 @@
         <v>12</v>
       </c>
       <c r="AD3" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="AE3" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="AG3" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="AH3" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="AI3" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="AJ3" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="AK3" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="AL3" t="s">
         <v>14</v>
       </c>
       <c r="AM3" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="AN3" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:42" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="B4">
         <v>120753969</v>
       </c>
       <c r="C4" t="s">
-        <v>21</v>
+        <v>94</v>
       </c>
       <c r="D4" t="s">
-        <v>22</v>
+        <v>94</v>
       </c>
       <c r="E4" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="F4" t="s">
         <v>15</v>
       </c>
       <c r="G4" t="s">
+        <v>94</v>
+      </c>
+      <c r="H4" t="s">
+        <v>18</v>
+      </c>
+      <c r="I4" t="s">
+        <v>30</v>
+      </c>
+      <c r="J4" t="s">
+        <v>34</v>
+      </c>
+      <c r="M4" t="s">
         <v>16</v>
       </c>
-      <c r="H4" t="s">
-        <v>23</v>
-      </c>
-      <c r="I4" t="s">
-        <v>35</v>
-      </c>
-      <c r="J4" t="s">
-        <v>39</v>
-      </c>
-      <c r="M4" t="s">
-        <v>17</v>
-      </c>
       <c r="N4" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="O4" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="P4" t="s">
-        <v>23</v>
+        <v>94</v>
       </c>
       <c r="Q4" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="R4" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="S4" s="1">
-        <v>61.7</v>
+        <v>300</v>
       </c>
       <c r="T4" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="U4" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="V4" s="1">
         <v>34.189189189189193</v>
       </c>
       <c r="W4" s="1" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="X4" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="Y4" t="s">
         <v>13</v>
@@ -1117,102 +1102,102 @@
         <v>12</v>
       </c>
       <c r="AD4" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="AE4" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="AG4" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="AH4" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="AI4" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="AJ4" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="AK4" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="AL4" t="s">
         <v>14</v>
       </c>
       <c r="AM4" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="AN4" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="B5">
         <v>120753968</v>
       </c>
       <c r="C5" t="s">
-        <v>83</v>
+        <v>95</v>
       </c>
       <c r="D5" t="s">
-        <v>84</v>
+        <v>95</v>
       </c>
       <c r="E5" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="F5" t="s">
         <v>15</v>
       </c>
       <c r="G5" t="s">
+        <v>95</v>
+      </c>
+      <c r="H5" t="s">
+        <v>77</v>
+      </c>
+      <c r="I5" t="s">
+        <v>30</v>
+      </c>
+      <c r="J5" t="s">
+        <v>34</v>
+      </c>
+      <c r="M5" t="s">
         <v>16</v>
       </c>
-      <c r="H5" t="s">
-        <v>86</v>
-      </c>
-      <c r="I5" t="s">
-        <v>35</v>
-      </c>
-      <c r="J5" t="s">
-        <v>39</v>
-      </c>
-      <c r="M5" t="s">
-        <v>17</v>
-      </c>
       <c r="N5" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="O5" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="P5" t="s">
-        <v>86</v>
+        <v>95</v>
       </c>
       <c r="Q5" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="R5" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="S5" s="1">
-        <v>57.8</v>
+        <v>400</v>
       </c>
       <c r="T5" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="U5" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="V5" s="5" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="W5" s="1" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="X5" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="Y5" t="s">
         <v>13</v>
@@ -1227,99 +1212,105 @@
         <v>12</v>
       </c>
       <c r="AD5" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="AE5" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="AG5" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="AH5" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="AI5" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="AJ5" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="AK5" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="AL5" t="s">
         <v>12</v>
       </c>
       <c r="AM5" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="AN5" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="B6">
         <v>123456789</v>
       </c>
       <c r="C6" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="D6" t="s">
-        <v>101</v>
+        <v>96</v>
+      </c>
+      <c r="E6" t="s">
+        <v>76</v>
       </c>
       <c r="F6" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="G6" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="H6" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="I6" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="J6" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="M6" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="N6" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="O6" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="P6" t="s">
-        <v>101</v>
+        <v>96</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>26</v>
       </c>
       <c r="R6" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="S6" s="1">
-        <v>63.18</v>
+        <v>500</v>
       </c>
       <c r="T6" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="U6" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="V6" s="1">
         <v>36.861111111111114</v>
       </c>
       <c r="W6" s="1" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="X6" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="Y6" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="Z6" t="s">
         <v>12</v>
@@ -1331,34 +1322,34 @@
         <v>12</v>
       </c>
       <c r="AD6" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="AE6" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="AG6" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="AH6" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="AI6" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="AJ6" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
       <c r="AK6" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
       <c r="AL6" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="AM6" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="AN6" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>